<commit_message>
added springer url crawler
</commit_message>
<xml_diff>
--- a/url crawler/europePMC/csv/europePMC_test.xlsx
+++ b/url crawler/europePMC/csv/europePMC_test.xlsx
@@ -14,12 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="45">
   <si>
     <t xml:space="preserve">Keyword : </t>
   </si>
   <si>
-    <t>https://europepmc.org/search?query=plant%20breeding</t>
+    <t>https://europepmc.org/search?query=car</t>
   </si>
   <si>
     <t xml:space="preserve">Database : </t>
@@ -31,7 +31,7 @@
     <t xml:space="preserve">Date : </t>
   </si>
   <si>
-    <t>2018-08-02T10:34:59.310710</t>
+    <t>2018-08-24T11:12:13.832042</t>
   </si>
   <si>
     <t>S.No</t>
@@ -70,148 +70,85 @@
     <t>1</t>
   </si>
   <si>
-    <t>https://europepmc.org/abstract/MED/29681742;jsessionid=E4A9B5CC7873DA8C1CFD52E143D03D92</t>
-  </si>
-  <si>
-    <t>Single Nucleotide Polymorphisms in the HIRA Gene Affect Litter Size in Small Tail Han Sheep.</t>
-  </si>
-  <si>
-    <t>Animals : an Open Access Journal From MDPI</t>
-  </si>
-  <si>
-    <t>[04 May 2018, 8(5)]</t>
-  </si>
-  <si>
-    <t>10.3390/ani8050071</t>
-  </si>
-  <si>
-    <t>Mei Zhou</t>
-  </si>
-  <si>
-    <t>Key Laboratory of Animal Genetics and Breeding and Reproduction of Ministry of Agriculture, Institute of Animal Science, Chinese Academy of Agricultural Sciences, Beijing 100193, China. 1229zhoumei@163.com.</t>
-  </si>
-  <si>
-    <t>China</t>
-  </si>
-  <si>
-    <t>1229zhoumei@163.com</t>
-  </si>
-  <si>
-    <t>Zhangyuan Pan</t>
-  </si>
-  <si>
-    <t>Key Laboratory of Animal Genetics and Breeding and Reproduction of Ministry of Agriculture, Institute of Animal Science, Chinese Academy of Agricultural Sciences, Beijing 100193, China. pzq170450077@163.com.</t>
-  </si>
-  <si>
-    <t>pzq170450077@163.com</t>
-  </si>
-  <si>
-    <t>Xiaohan Cao</t>
-  </si>
-  <si>
-    <t>Key Laboratory of Animal Genetics and Breeding and Reproduction of Ministry of Agriculture, Institute of Animal Science, Chinese Academy of Agricultural Sciences, Beijing 100193, China. caoxiaohan2007@hotmail.com.</t>
-  </si>
-  <si>
-    <t>caoxiaohan2007@hotmail.com</t>
-  </si>
-  <si>
-    <t>Xiaofei Guo</t>
-  </si>
-  <si>
-    <t>Key Laboratory of Animal Genetics and Breeding and Reproduction of Ministry of Agriculture, Institute of Animal Science, Chinese Academy of Agricultural Sciences, Beijing 100193, China. guoxfnongda@163.com.</t>
-  </si>
-  <si>
-    <t>guoxfnongda@163.com</t>
-  </si>
-  <si>
-    <t>Xiaoyun He</t>
-  </si>
-  <si>
-    <t>Key Laboratory of Animal Genetics and Breeding and Reproduction of Ministry of Agriculture, Institute of Animal Science, Chinese Academy of Agricultural Sciences, Beijing 100193, China. hedayun@sina.cn.</t>
-  </si>
-  <si>
-    <t>hedayun@sina.cn</t>
-  </si>
-  <si>
-    <t>Qing Sun</t>
-  </si>
-  <si>
-    <t>Key Laboratory of Animal Genetics and Breeding and Reproduction of Ministry of Agriculture, Institute of Animal Science, Chinese Academy of Agricultural Sciences, Beijing 100193, China. sunqing0514@sina.com.</t>
-  </si>
-  <si>
-    <t>sunqing0514@sina.com</t>
-  </si>
-  <si>
-    <t>Ran Di</t>
-  </si>
-  <si>
-    <t>Key Laboratory of Animal Genetics and Breeding and Reproduction of Ministry of Agriculture, Institute of Animal Science, Chinese Academy of Agricultural Sciences, Beijing 100193, China. dirangirl@163.com.</t>
-  </si>
-  <si>
-    <t>dirangirl@163.com</t>
-  </si>
-  <si>
-    <t>Wenping Hu</t>
-  </si>
-  <si>
-    <t>Key Laboratory of Animal Genetics and Breeding and Reproduction of Ministry of Agriculture, Institute of Animal Science, Chinese Academy of Agricultural Sciences, Beijing 100193, China. pinkyhoho@163.com.</t>
-  </si>
-  <si>
-    <t>pinkyhoho@163.com</t>
-  </si>
-  <si>
-    <t>Xiangyu Wang</t>
-  </si>
-  <si>
-    <t>Key Laboratory of Animal Genetics and Breeding and Reproduction of Ministry of Agriculture, Institute of Animal Science, Chinese Academy of Agricultural Sciences, Beijing 100193, China. xiangyu_wiggle@163.com.</t>
-  </si>
-  <si>
-    <t>xiangyu_wiggle@163.com</t>
-  </si>
-  <si>
-    <t>Xiaosheng Zhang</t>
-  </si>
-  <si>
-    <t>Tianjin Institute of Animal Sciences, Tianjin 300381, China. zhangxs0221@126.com.</t>
-  </si>
-  <si>
-    <t>zhangxs0221@126.com</t>
-  </si>
-  <si>
-    <t>Jinlong Zhang</t>
-  </si>
-  <si>
-    <t>Tianjin Institute of Animal Sciences, Tianjin 300381, China. jlzhang1010@163.com.</t>
-  </si>
-  <si>
-    <t>jlzhang1010@163.com</t>
-  </si>
-  <si>
-    <t>Chunyuan Zhang</t>
-  </si>
-  <si>
-    <t>State Key Laboratory for Agrobiotechnology, College of Biological Sciences, China Agricultural University, Beijing 100193, China. dachunyuanzi@cau.edu.cn.</t>
-  </si>
-  <si>
-    <t>dachunyuanzi@cau.edu</t>
-  </si>
-  <si>
-    <t>Qiuyue Liu</t>
-  </si>
-  <si>
-    <t>Key Laboratory of Animal Genetics and Breeding and Reproduction of Ministry of Agriculture, Institute of Animal Science, Chinese Academy of Agricultural Sciences, Beijing 100193, China. mxchu@263.net.</t>
-  </si>
-  <si>
-    <t>mxchu@263.net</t>
-  </si>
-  <si>
-    <t>Mingxing Chu</t>
-  </si>
-  <si>
-    <t>Key Laboratory of Animal Genetics and Breeding and Reproduction of Ministry of Agriculture, Institute of Animal Science, Chinese Academy of Agricultural Sciences, Beijing 100193, China. liuqiuyue@caas.cn.</t>
-  </si>
-  <si>
-    <t>liuqiuyue@caas.cn</t>
+    <t>https://europepmc.org/abstract/MED/30097654;jsessionid=FFFE6976C99B501827D8051427E36BB5</t>
+  </si>
+  <si>
+    <t>Use of car beds for infant travel: a review of the literature.</t>
+  </si>
+  <si>
+    <t>Journal of Perinatology : Official Journal of the California Perinatal Association</t>
+  </si>
+  <si>
+    <t>[10 Aug 2018]</t>
+  </si>
+  <si>
+    <t>10.1038/s41372-018-0195-7</t>
+  </si>
+  <si>
+    <t>Natalie Davis</t>
+  </si>
+  <si>
+    <t>University of Maryland School of Medicine</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Cannot get email</t>
+  </si>
+  <si>
+    <t>Nina Shah</t>
+  </si>
+  <si>
+    <t>Division of Neonatology, University of Maryland Children's Hospital, University of Maryland School of Medicine, Baltimore, MD, USA.</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>https://europepmc.org/abstract/MED/29370379;jsessionid=FFFE6976C99B501827D8051427E36BB5</t>
+  </si>
+  <si>
+    <t>Glycan-directed CAR-T cells.</t>
+  </si>
+  <si>
+    <t>Glycobiology</t>
+  </si>
+  <si>
+    <t>[01 Sep 2018, 28(9):656-669]</t>
+  </si>
+  <si>
+    <t>10.1093/glycob/cwy008</t>
+  </si>
+  <si>
+    <t>Catharina Steentoft</t>
+  </si>
+  <si>
+    <t>Copenhagen Center for Glycomics, Departments of Cellular and Molecular Medicine and Odontology, Faculty of Health Sciences, University of Copenhagen, Copenhagen, Denmark.</t>
+  </si>
+  <si>
+    <t>Denmark</t>
+  </si>
+  <si>
+    <t>Denis Migliorini</t>
+  </si>
+  <si>
+    <t>Center of Cellular Immunotherapies, Abramson Cancer Center and the Department of Pathology and Laboratory Medicine, Perelman School of Medicine, University of Pennsylvania, Philadelphia, PA, USA.</t>
+  </si>
+  <si>
+    <t>Tiffany R King</t>
+  </si>
+  <si>
+    <t>Ulla Mandel</t>
+  </si>
+  <si>
+    <t>Carl H June</t>
+  </si>
+  <si>
+    <t>Avery D Posey</t>
   </si>
 </sst>
 </file>
@@ -556,7 +493,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -661,84 +598,85 @@
         <v>27</v>
       </c>
       <c r="H6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="I6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="J6" t="s">
         <v>28</v>
       </c>
       <c r="K6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11">
-      <c r="G7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" t="s">
         <v>30</v>
       </c>
-      <c r="H7" t="s">
+      <c r="B8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" t="s">
         <v>32</v>
       </c>
-      <c r="I7" t="s">
-        <v>32</v>
-      </c>
-      <c r="J7" t="s">
-        <v>31</v>
-      </c>
-      <c r="K7" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="D8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E8" t="s">
+        <v>34</v>
+      </c>
+      <c r="F8" t="s">
+        <v>35</v>
+      </c>
       <c r="G8" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H8" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="I8" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="J8" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="K8" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:11">
       <c r="G9" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="H9" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="I9" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="J9" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="K9" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:11">
       <c r="G10" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="H10" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="I10" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="J10" t="s">
         <v>40</v>
       </c>
       <c r="K10" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -746,135 +684,50 @@
         <v>42</v>
       </c>
       <c r="H11" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="I11" t="s">
-        <v>44</v>
+        <v>26</v>
       </c>
       <c r="J11" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="K11" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:11">
       <c r="G12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H12" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="I12" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="J12" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="K12" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:11">
       <c r="G13" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="H13" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="I13" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="J13" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="K13" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11">
-      <c r="G14" t="s">
-        <v>51</v>
-      </c>
-      <c r="H14" t="s">
-        <v>53</v>
-      </c>
-      <c r="I14" t="s">
-        <v>53</v>
-      </c>
-      <c r="J14" t="s">
-        <v>52</v>
-      </c>
-      <c r="K14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11">
-      <c r="G15" t="s">
-        <v>54</v>
-      </c>
-      <c r="H15" t="s">
-        <v>56</v>
-      </c>
-      <c r="I15" t="s">
-        <v>56</v>
-      </c>
-      <c r="J15" t="s">
-        <v>55</v>
-      </c>
-      <c r="K15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11">
-      <c r="G16" t="s">
-        <v>57</v>
-      </c>
-      <c r="H16" t="s">
-        <v>59</v>
-      </c>
-      <c r="I16" t="s">
-        <v>59</v>
-      </c>
-      <c r="J16" t="s">
-        <v>58</v>
-      </c>
-      <c r="K16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="7:11">
-      <c r="G17" t="s">
-        <v>60</v>
-      </c>
-      <c r="H17" t="s">
-        <v>62</v>
-      </c>
-      <c r="I17" t="s">
-        <v>62</v>
-      </c>
-      <c r="J17" t="s">
-        <v>61</v>
-      </c>
-      <c r="K17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="7:11">
-      <c r="G18" t="s">
-        <v>63</v>
-      </c>
-      <c r="H18" t="s">
-        <v>65</v>
-      </c>
-      <c r="I18" t="s">
-        <v>65</v>
-      </c>
-      <c r="J18" t="s">
-        <v>64</v>
-      </c>
-      <c r="K18" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -882,6 +735,7 @@
     <hyperlink ref="B1" r:id="rId1"/>
     <hyperlink ref="B2" r:id="rId2"/>
     <hyperlink ref="B5" r:id="rId3"/>
+    <hyperlink ref="B8" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>